<commit_message>
Nearly all technical details are finished!
</commit_message>
<xml_diff>
--- a/first/staticroot/dogs_data.xlsx
+++ b/first/staticroot/dogs_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fgoncharov/PycharmProjects/PetMates/first/staticroot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726288C5-3D5D-1046-8209-971DB65CCBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B64417D-586D-2044-ACFE-4138F439F2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{89B0CB10-1F7B-BE40-8EFE-DEA173D7CA3C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" xr2:uid="{89B0CB10-1F7B-BE40-8EFE-DEA173D7CA3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -231,9 +231,6 @@
     <t>Далматин</t>
   </si>
   <si>
-    <t>Компаньон/Сторожевая/Охотничая</t>
-  </si>
-  <si>
     <t>Короткошерстный</t>
   </si>
   <si>
@@ -247,6 +244,9 @@
   </si>
   <si>
     <t>Нет</t>
+  </si>
+  <si>
+    <t>Тип поведения</t>
   </si>
 </sst>
 </file>
@@ -658,7 +658,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="P47" sqref="P47"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -679,7 +679,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>31</v>
@@ -723,7 +723,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" s="6">
         <v>64</v>
@@ -750,7 +750,7 @@
         <v>5</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M2" s="7">
         <v>2</v>
@@ -764,7 +764,7 @@
         <v>61</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="6">
         <v>60</v>
@@ -791,7 +791,7 @@
         <v>3</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M3" s="7">
         <v>5</v>
@@ -805,7 +805,7 @@
         <v>61</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="6">
         <v>32</v>
@@ -832,7 +832,7 @@
         <v>1</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M4" s="7">
         <v>4</v>
@@ -846,7 +846,7 @@
         <v>62</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="6">
         <v>62</v>
@@ -873,7 +873,7 @@
         <v>5</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M5" s="7">
         <v>4</v>
@@ -887,7 +887,7 @@
         <v>60</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="6">
         <v>37</v>
@@ -914,7 +914,7 @@
         <v>4</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M6" s="7">
         <v>3</v>
@@ -928,7 +928,7 @@
         <v>61</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" s="6">
         <v>27</v>
@@ -955,7 +955,7 @@
         <v>3</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M7" s="7">
         <v>5</v>
@@ -969,7 +969,7 @@
         <v>62</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" s="6">
         <v>57</v>
@@ -996,7 +996,7 @@
         <v>5</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M8" s="7">
         <v>5</v>
@@ -1010,7 +1010,7 @@
         <v>61</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="6">
         <v>19</v>
@@ -1037,7 +1037,7 @@
         <v>4</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M9" s="7">
         <v>2</v>
@@ -1051,7 +1051,7 @@
         <v>61</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="6">
         <v>55</v>
@@ -1078,7 +1078,7 @@
         <v>5</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M10" s="7">
         <v>5</v>
@@ -1092,7 +1092,7 @@
         <v>61</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="6">
         <v>28</v>
@@ -1119,7 +1119,7 @@
         <v>5</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M11" s="7">
         <v>5</v>
@@ -1133,7 +1133,7 @@
         <v>62</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="6">
         <v>70</v>
@@ -1160,7 +1160,7 @@
         <v>5</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M12" s="7">
         <v>4</v>
@@ -1174,7 +1174,7 @@
         <v>61</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="6">
         <v>57</v>
@@ -1201,7 +1201,7 @@
         <v>3</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M13" s="7">
         <v>3</v>
@@ -1215,7 +1215,7 @@
         <v>60</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="6">
         <v>28</v>
@@ -1242,7 +1242,7 @@
         <v>5</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M14" s="7">
         <v>5</v>
@@ -1256,7 +1256,7 @@
         <v>62</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="6">
         <v>68</v>
@@ -1283,7 +1283,7 @@
         <v>5</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M15" s="7">
         <v>2</v>
@@ -1297,7 +1297,7 @@
         <v>62</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16" s="6">
         <v>83</v>
@@ -1324,7 +1324,7 @@
         <v>5</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M16" s="7">
         <v>4</v>
@@ -1338,7 +1338,7 @@
         <v>61</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="6">
         <v>16</v>
@@ -1365,7 +1365,7 @@
         <v>4</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M17" s="7">
         <v>5</v>
@@ -1379,7 +1379,7 @@
         <v>62</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" s="6">
         <v>71</v>
@@ -1406,7 +1406,7 @@
         <v>5</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M18" s="7">
         <v>5</v>
@@ -1420,7 +1420,7 @@
         <v>61</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" s="6">
         <v>30</v>
@@ -1447,7 +1447,7 @@
         <v>3</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M19" s="7">
         <v>3</v>
@@ -1461,7 +1461,7 @@
         <v>60</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" s="6">
         <v>32</v>
@@ -1488,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M20" s="7">
         <v>5</v>
@@ -1502,7 +1502,7 @@
         <v>61</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="6">
         <v>58</v>
@@ -1529,7 +1529,7 @@
         <v>2</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M21" s="7">
         <v>5</v>
@@ -1543,7 +1543,7 @@
         <v>62</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22" s="6">
         <v>74</v>
@@ -1570,7 +1570,7 @@
         <v>5</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M22" s="7">
         <v>4</v>
@@ -1584,7 +1584,7 @@
         <v>61</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="6">
         <v>23</v>
@@ -1611,7 +1611,7 @@
         <v>1</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M23" s="7">
         <v>4</v>
@@ -1625,7 +1625,7 @@
         <v>62</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D24" s="6">
         <v>68</v>
@@ -1652,7 +1652,7 @@
         <v>5</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M24" s="7">
         <v>3</v>
@@ -1666,7 +1666,7 @@
         <v>61</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D25" s="6">
         <v>30</v>
@@ -1693,7 +1693,7 @@
         <v>4</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M25" s="7">
         <v>5</v>
@@ -1707,7 +1707,7 @@
         <v>62</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="6">
         <v>73</v>
@@ -1734,7 +1734,7 @@
         <v>5</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M26" s="7">
         <v>4</v>
@@ -1748,7 +1748,7 @@
         <v>62</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" s="6">
         <v>60</v>
@@ -1775,7 +1775,7 @@
         <v>5</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M27" s="7">
         <v>5</v>
@@ -1789,7 +1789,7 @@
         <v>61</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D28" s="6">
         <v>24</v>
@@ -1816,7 +1816,7 @@
         <v>5</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M28" s="7">
         <v>5</v>
@@ -1830,7 +1830,7 @@
         <v>61</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29" s="6">
         <v>20</v>
@@ -1857,7 +1857,7 @@
         <v>4</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M29" s="7">
         <v>2</v>
@@ -1871,7 +1871,7 @@
         <v>61</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D30" s="6">
         <v>55</v>
@@ -1898,7 +1898,7 @@
         <v>2</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M30" s="7">
         <v>5</v>
@@ -1912,7 +1912,7 @@
         <v>62</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D31" s="6">
         <v>65</v>
@@ -1939,7 +1939,7 @@
         <v>5</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M31" s="7">
         <v>4</v>
@@ -1953,7 +1953,7 @@
         <v>62</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D32" s="6">
         <v>65</v>
@@ -1980,7 +1980,7 @@
         <v>5</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M32" s="7">
         <v>3</v>
@@ -1994,7 +1994,7 @@
         <v>60</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D33" s="6">
         <v>65</v>
@@ -2021,7 +2021,7 @@
         <v>1</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M33" s="7">
         <v>4</v>
@@ -2035,7 +2035,7 @@
         <v>62</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D34" s="6">
         <v>53</v>
@@ -2062,7 +2062,7 @@
         <v>2</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M34" s="7">
         <v>4</v>
@@ -2076,7 +2076,7 @@
         <v>62</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D35" s="6">
         <v>75</v>
@@ -2103,7 +2103,7 @@
         <v>5</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M35" s="7">
         <v>5</v>
@@ -2117,7 +2117,7 @@
         <v>60</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D36" s="6">
         <v>65</v>
@@ -2144,7 +2144,7 @@
         <v>3</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M36" s="7">
         <v>4</v>
@@ -2158,7 +2158,7 @@
         <v>61</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D37" s="6">
         <v>38</v>
@@ -2185,7 +2185,7 @@
         <v>3</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M37" s="7">
         <v>5</v>
@@ -2199,7 +2199,7 @@
         <v>61</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D38" s="6">
         <v>27</v>
@@ -2226,7 +2226,7 @@
         <v>4</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M38" s="7">
         <v>5</v>
@@ -2240,7 +2240,7 @@
         <v>62</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D39" s="6">
         <v>78</v>
@@ -2267,7 +2267,7 @@
         <v>5</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M39" s="7">
         <v>4</v>
@@ -2281,7 +2281,7 @@
         <v>61</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D40" s="6">
         <v>30</v>
@@ -2308,7 +2308,7 @@
         <v>2</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M40" s="7">
         <v>5</v>
@@ -2322,7 +2322,7 @@
         <v>62</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D41" s="6">
         <v>74</v>
@@ -2349,7 +2349,7 @@
         <v>5</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M41" s="7">
         <v>4</v>
@@ -2363,7 +2363,7 @@
         <v>61</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D42" s="6">
         <v>24</v>
@@ -2390,7 +2390,7 @@
         <v>3</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M42" s="7">
         <v>5</v>
@@ -2404,7 +2404,7 @@
         <v>61</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D43" s="6">
         <v>56</v>
@@ -2431,7 +2431,7 @@
         <v>1</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M43" s="7">
         <v>5</v>
@@ -2445,7 +2445,7 @@
         <v>61</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D44" s="6">
         <v>25</v>
@@ -2472,7 +2472,7 @@
         <v>3</v>
       </c>
       <c r="L44" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M44" s="7">
         <v>5</v>
@@ -2486,7 +2486,7 @@
         <v>61</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D45" s="6">
         <v>18</v>
@@ -2513,7 +2513,7 @@
         <v>1</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M45" s="7">
         <v>1</v>
@@ -2527,7 +2527,7 @@
         <v>62</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D46" s="6">
         <v>37</v>
@@ -2554,7 +2554,7 @@
         <v>5</v>
       </c>
       <c r="L46" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M46" s="7">
         <v>4</v>
@@ -2568,7 +2568,7 @@
         <v>61</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D47" s="6">
         <v>24</v>
@@ -2595,7 +2595,7 @@
         <v>4</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M47" s="7">
         <v>5</v>
@@ -2609,7 +2609,7 @@
         <v>61</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D48" s="6">
         <v>20</v>
@@ -2636,7 +2636,7 @@
         <v>3</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M48" s="7">
         <v>4</v>
@@ -2650,7 +2650,7 @@
         <v>62</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D49" s="6">
         <v>58</v>
@@ -2677,7 +2677,7 @@
         <v>5</v>
       </c>
       <c r="L49" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M49" s="7">
         <v>5</v>
@@ -2691,7 +2691,7 @@
         <v>61</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D50" s="6">
         <v>24</v>
@@ -2718,7 +2718,7 @@
         <v>1</v>
       </c>
       <c r="L50" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M50" s="7">
         <v>5</v>

</xml_diff>